<commit_message>
add contrast response analysis
</commit_message>
<xml_diff>
--- a/result_table_templates/ContrastResponse_CA.xlsx
+++ b/result_table_templates/ContrastResponse_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregschwartz/matlab/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E0AA20-C950-7A4D-959C-56935DBF72C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCA8E3-5FD6-664F-9DEC-8E9B2F723A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17260" yWindow="860" windowWidth="17040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="231" zoomScaleNormal="231" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>